<commit_message>
fixed error Damien made in excel. And removed logger lines
</commit_message>
<xml_diff>
--- a/static/excel/DB_Const_valide_sat_xyz_RTN.xlsx
+++ b/static/excel/DB_Const_valide_sat_xyz_RTN.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon.Andersson\PycharmProjects\untitled\web2py\applications\linkbudgetweb\static\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1425" windowWidth="22995" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="VSAT" sheetId="1" r:id="rId1"/>
@@ -237,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="12">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;deg&quot;"/>
     <numFmt numFmtId="165" formatCode="0\ &quot;kms&quot;"/>
@@ -1002,6 +1007,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1049,7 +1057,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1082,9 +1090,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1117,6 +1142,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1296,7 +1338,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3043,8 +3085,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3094,10 +3136,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>99</v>
-      </c>
-      <c r="E2">
-        <v>99</v>
+        <v>0.99</v>
+      </c>
+      <c r="E2" s="40">
+        <v>0.99</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3123,10 +3165,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E3" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F3" s="40">
         <v>1</v>
@@ -3152,10 +3194,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E4" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F4" s="40">
         <v>1</v>
@@ -3181,10 +3223,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E5" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F5" s="40">
         <v>1</v>
@@ -3210,10 +3252,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E6" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F6" s="40">
         <v>1</v>
@@ -3239,10 +3281,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E7" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F7" s="40">
         <v>1</v>
@@ -3268,10 +3310,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E8" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F8" s="40">
         <v>1</v>
@@ -3297,10 +3339,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E9" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F9" s="40">
         <v>1</v>
@@ -3326,10 +3368,10 @@
         <v>0</v>
       </c>
       <c r="D10" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E10" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F10" s="40">
         <v>1</v>
@@ -3355,10 +3397,10 @@
         <v>0</v>
       </c>
       <c r="D11" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E11" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F11" s="40">
         <v>1</v>
@@ -3384,10 +3426,10 @@
         <v>0</v>
       </c>
       <c r="D12" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E12" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F12" s="40">
         <v>1</v>
@@ -3413,10 +3455,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E13" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F13" s="40">
         <v>1</v>
@@ -3442,10 +3484,10 @@
         <v>0</v>
       </c>
       <c r="D14" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E14" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F14" s="40">
         <v>1</v>
@@ -3471,10 +3513,10 @@
         <v>0</v>
       </c>
       <c r="D15" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E15" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F15" s="40">
         <v>1</v>
@@ -3500,10 +3542,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E16" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F16" s="40">
         <v>1</v>
@@ -3529,10 +3571,10 @@
         <v>0</v>
       </c>
       <c r="D17" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="E17" s="40">
-        <v>99</v>
+        <v>0.99</v>
       </c>
       <c r="F17" s="40">
         <v>1</v>

</xml_diff>